<commit_message>
Initial upload of functional code
</commit_message>
<xml_diff>
--- a/Preprocessing/Data/ModENCODE Worm RNA-Seq Datasets.xlsx
+++ b/Preprocessing/Data/ModENCODE Worm RNA-Seq Datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astra/Documents/GitHub/Caenorhabditis_RNAseq_Browser/Preprocessing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF24FDC-91D0-A841-A4E0-F1D984674465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936AD564-2AAE-2D4C-9C51-CC64080A48DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="4180" windowWidth="26840" windowHeight="15940" xr2:uid="{3919414E-38FC-8245-8A4F-C65263295AE0}"/>
   </bookViews>
@@ -2016,13 +2016,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5924D8B-669F-384F-B291-C29A3E2AF327}">
   <dimension ref="A1:S166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="43" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Preprocessing and analysis of embryonic timecourse data
</commit_message>
<xml_diff>
--- a/Preprocessing/Data/ModENCODE Worm RNA-Seq Datasets.xlsx
+++ b/Preprocessing/Data/ModENCODE Worm RNA-Seq Datasets.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astra/Documents/GitHub/Caenorhabditis_RNAseq_Browser/Preprocessing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936AD564-2AAE-2D4C-9C51-CC64080A48DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E5F0A0-2A52-0C47-BF68-EBF64D396D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="4180" windowWidth="26840" windowHeight="15940" xr2:uid="{3919414E-38FC-8245-8A4F-C65263295AE0}"/>
+    <workbookView xWindow="9560" yWindow="980" windowWidth="26840" windowHeight="15940" xr2:uid="{3919414E-38FC-8245-8A4F-C65263295AE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Worm RNA-Seq Datasets" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2016,13 +2016,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5924D8B-669F-384F-B291-C29A3E2AF327}">
   <dimension ref="A1:S166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
     <col min="4" max="4" width="81.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Major update to restructure/revise analysis options for different species.
</commit_message>
<xml_diff>
--- a/Preprocessing/Data/ModENCODE Worm RNA-Seq Datasets.xlsx
+++ b/Preprocessing/Data/ModENCODE Worm RNA-Seq Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astra/Documents/GitHub/Caenorhabditis_RNAseq_Browser/Preprocessing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E5F0A0-2A52-0C47-BF68-EBF64D396D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23C03CE-9CC7-E247-8442-19DC81ECB239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="980" windowWidth="26840" windowHeight="15940" xr2:uid="{3919414E-38FC-8245-8A4F-C65263295AE0}"/>
+    <workbookView xWindow="36240" yWindow="7140" windowWidth="26840" windowHeight="15940" xr2:uid="{3919414E-38FC-8245-8A4F-C65263295AE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Worm RNA-Seq Datasets" sheetId="1" r:id="rId1"/>
@@ -2016,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5924D8B-669F-384F-B291-C29A3E2AF327}">
   <dimension ref="A1:S166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2025,6 +2025,7 @@
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="39.5" customWidth="1"/>
     <col min="4" max="4" width="81.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="43" x14ac:dyDescent="0.2">

</xml_diff>